<commit_message>
feat: some features added
</commit_message>
<xml_diff>
--- a/EmptyAPI/EmptyAPI/wwwroot/Datas-17.August.2022.xlsx
+++ b/EmptyAPI/EmptyAPI/wwwroot/Datas-17.August.2022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Type</t>
   </si>
@@ -29,19 +29,22 @@
     <t>Profit</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>United States of America</t>
+    <t>Amarilla</t>
+  </si>
+  <si>
+    <t>Carretera</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Paseo</t>
+  </si>
+  <si>
+    <t>Velo</t>
+  </si>
+  <si>
+    <t>VTT</t>
   </si>
 </sst>
 </file>
@@ -87,7 +90,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -115,16 +118,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="0">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="C2" s="0">
-        <v>24887654.884999987</v>
+        <v>17747116.06</v>
       </c>
       <c r="D2" s="0">
-        <v>2044508.615</v>
+        <v>1290163.4400000002</v>
       </c>
       <c r="E2" s="0">
-        <v>3529228.8850000007</v>
+        <v>2814104.0600000005</v>
       </c>
     </row>
     <row r="3">
@@ -132,16 +135,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="0">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="C3" s="0">
-        <v>24354172.28000001</v>
+        <v>13815307.885000002</v>
       </c>
       <c r="D3" s="0">
-        <v>1727502.2199999997</v>
+        <v>1122212.6149999998</v>
       </c>
       <c r="E3" s="0">
-        <v>3781020.7799999993</v>
+        <v>1826804.885</v>
       </c>
     </row>
     <row r="4">
@@ -149,16 +152,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="0">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="C4" s="0">
-        <v>23505340.819999997</v>
+        <v>15390801.880000003</v>
       </c>
       <c r="D4" s="0">
-        <v>1416126.68</v>
+        <v>1159032.62</v>
       </c>
       <c r="E4" s="0">
-        <v>3680388.8199999994</v>
+        <v>2114754.8799999994</v>
       </c>
     </row>
     <row r="5">
@@ -166,16 +169,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="0">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="C5" s="0">
-        <v>20949352.11</v>
+        <v>33011143.95000001</v>
       </c>
       <c r="D5" s="0">
-        <v>1777582.8900000001</v>
+        <v>2600518.0499999993</v>
       </c>
       <c r="E5" s="0">
-        <v>2907523.110000001</v>
+        <v>4797437.95</v>
       </c>
     </row>
     <row r="6">
@@ -183,16 +186,33 @@
         <v>9</v>
       </c>
       <c r="B6" s="0">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="C6" s="0">
-        <v>25029830.165</v>
+        <v>18250059.465</v>
       </c>
       <c r="D6" s="0">
-        <v>2239527.835</v>
+        <v>1576709.035</v>
       </c>
       <c r="E6" s="0">
-        <v>2995540.665</v>
+        <v>2305992.4650000003</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0">
+        <v>109</v>
+      </c>
+      <c r="C7" s="0">
+        <v>20511921.019999996</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1456612.4800000002</v>
+      </c>
+      <c r="E7" s="0">
+        <v>3034608.0200000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>